<commit_message>
update new tap stock
</commit_message>
<xml_diff>
--- a/stocks/new_tap_stock.xlsx
+++ b/stocks/new_tap_stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\sync_ck\stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F61E62-9E42-4A62-BDFE-A453F3AE93B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B980927-6CCB-460E-ACCE-FC852507C528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A17BD16-390E-426D-8CA1-F70AD4237B33}"/>
   </bookViews>
@@ -1702,13 +1702,13 @@
     <t>7C98-1149-3W</t>
   </si>
   <si>
-    <t>PARTNO</t>
-  </si>
-  <si>
-    <t>CTN</t>
-  </si>
-  <si>
-    <t>QTY</t>
+    <t>part_no</t>
+  </si>
+  <si>
+    <t>qty</t>
+  </si>
+  <si>
+    <t>ctn</t>
   </si>
 </sst>
 </file>
@@ -2063,8 +2063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4C6EAE-635B-4F3A-87D3-FB612C4F9738}">
   <dimension ref="A1:C556"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A521" workbookViewId="0">
-      <selection activeCell="G537" sqref="G537"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2077,10 +2077,10 @@
         <v>555</v>
       </c>
       <c r="B1" t="s">
+        <v>556</v>
+      </c>
+      <c r="C1" t="s">
         <v>557</v>
-      </c>
-      <c r="C1" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>